<commit_message>
wrote methods that will parse an excel file and create a graph
</commit_message>
<xml_diff>
--- a/course_data/course_data.xlsx
+++ b/course_data/course_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>elec</t>
   </si>
@@ -33,10 +33,13 @@
     <t>math</t>
   </si>
   <si>
-    <t>mon</t>
-  </si>
-  <si>
-    <t>tues</t>
+    <t>MON</t>
+  </si>
+  <si>
+    <t>TUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -377,8 +380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,7 +391,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="C1">
         <v>201</v>
@@ -431,6 +434,15 @@
       <c r="C2">
         <v>201</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
@@ -450,6 +462,15 @@
       </c>
       <c r="C3">
         <v>202</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
started working on the python scraper
</commit_message>
<xml_diff>
--- a/course_data/course_data.xlsx
+++ b/course_data/course_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t>elec</t>
   </si>
@@ -40,6 +40,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>cpsc</t>
+  </si>
+  <si>
+    <t>WED</t>
+  </si>
+  <si>
+    <t>comm</t>
+  </si>
+  <si>
+    <t>D2B</t>
+  </si>
+  <si>
+    <t>FRI</t>
   </si>
 </sst>
 </file>
@@ -378,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,6 +504,64 @@
       </c>
       <c r="L3">
         <v>1900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>261</v>
+      </c>
+      <c r="C4">
+        <v>204</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>1200</v>
+      </c>
+      <c r="I4">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>280</v>
+      </c>
+      <c r="C5">
+        <v>201</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>2000</v>
+      </c>
+      <c r="I5">
+        <v>2100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new algorithm for graph coloring and finished the timetable component for GUI
</commit_message>
<xml_diff>
--- a/course_data/course_data.xlsx
+++ b/course_data/course_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="14">
   <si>
     <t>elec</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>FRI</t>
+  </si>
+  <si>
+    <t>THURS</t>
   </si>
 </sst>
 </file>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,31 +444,31 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="C2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H2">
-        <v>800</v>
+        <v>1900</v>
       </c>
       <c r="I2">
-        <v>900</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -473,10 +476,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>307</v>
+        <v>256</v>
       </c>
       <c r="C3">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -491,33 +494,24 @@
         <v>5</v>
       </c>
       <c r="H3">
-        <v>1300</v>
+        <v>800</v>
       </c>
       <c r="I3">
-        <v>1400</v>
-      </c>
-      <c r="J3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3">
-        <v>1800</v>
-      </c>
-      <c r="L3">
-        <v>1900</v>
+        <v>900</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>261</v>
+        <v>307</v>
       </c>
       <c r="C4">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -526,41 +520,79 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="I4">
-        <v>1300</v>
+        <v>1400</v>
+      </c>
+      <c r="J4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>1800</v>
+      </c>
+      <c r="L4">
+        <v>1900</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>261</v>
+      </c>
+      <c r="C5">
+        <v>204</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>1200</v>
+      </c>
+      <c r="I5">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>280</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>201</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
         <v>11</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>12</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>2000</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <v>2100</v>
       </c>
     </row>
@@ -571,12 +603,178 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>221</v>
+      </c>
+      <c r="C1">
+        <v>201</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>800</v>
+      </c>
+      <c r="I1">
+        <v>1200</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1">
+        <v>1000</v>
+      </c>
+      <c r="L1">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>256</v>
+      </c>
+      <c r="C2">
+        <v>201</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>800</v>
+      </c>
+      <c r="I2">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>307</v>
+      </c>
+      <c r="C3">
+        <v>202</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>1300</v>
+      </c>
+      <c r="I3">
+        <v>1400</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>1800</v>
+      </c>
+      <c r="L3">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>261</v>
+      </c>
+      <c r="C4">
+        <v>204</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>1200</v>
+      </c>
+      <c r="I4">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>280</v>
+      </c>
+      <c r="C5">
+        <v>201</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>2000</v>
+      </c>
+      <c r="I5">
+        <v>2100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>